<commit_message>
Added in main window for user input, stats sucessfully export to excel file.
Now its time to work on the game portion
</commit_message>
<xml_diff>
--- a/player_stats.xlsx
+++ b/player_stats.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,98 +436,154 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>KD</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Win percentage</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Top Agent</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Headshot Percentage</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Clutches</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>First Kills</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>First Deaths</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Knife Kills</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>149 Damage Done</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Rank</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Archetype</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1.05</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>PA1NT #Peak</t>
+        </is>
       </c>
       <c r="B2" t="n">
-        <v>48</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Iso</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>26.6</v>
+        <v>1.18</v>
+      </c>
+      <c r="C2" t="n">
+        <v>47</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
       </c>
       <c r="E2" t="n">
-        <v>42</v>
+        <v>33.5</v>
       </c>
       <c r="F2" t="n">
-        <v>156</v>
+        <v>47</v>
       </c>
       <c r="G2" t="n">
-        <v>153</v>
+        <v>486</v>
       </c>
       <c r="H2" t="n">
+        <v>446</v>
+      </c>
+      <c r="I2" t="n">
         <v>0</v>
       </c>
-      <c r="I2" t="n">
-        <v>3</v>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Nickel</t>
-        </is>
+      <c r="J2" t="n">
+        <v>29</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>['Engager', 'Rusher']</t>
+          <t>Lead</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>['Engager', 'Sniper', 'Rusher']</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>big bean #jakee</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="C3" t="n">
+        <v>46</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Clove</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>32.7</v>
+      </c>
+      <c r="F3" t="n">
+        <v>64</v>
+      </c>
+      <c r="G3" t="n">
+        <v>579</v>
+      </c>
+      <c r="H3" t="n">
+        <v>557</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>101</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Titanium</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>['Clutch King', 'Engager', 'Sniper', 'Rusher']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added in another tab for game history. Also new matches class for last 20 matches player has played.
Need to format data in game history tab. Also need to make sure that the specific game is loaded when a game is clicked on the game history tab
</commit_message>
<xml_diff>
--- a/player_stats.xlsx
+++ b/player_stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -587,6 +587,2030 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C4" t="n">
+        <v>57</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F4" t="n">
+        <v>14</v>
+      </c>
+      <c r="G4" t="n">
+        <v>138</v>
+      </c>
+      <c r="H4" t="n">
+        <v>156</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>15</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C5" t="n">
+        <v>57</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F5" t="n">
+        <v>14</v>
+      </c>
+      <c r="G5" t="n">
+        <v>138</v>
+      </c>
+      <c r="H5" t="n">
+        <v>156</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>15</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C6" t="n">
+        <v>57</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F6" t="n">
+        <v>14</v>
+      </c>
+      <c r="G6" t="n">
+        <v>138</v>
+      </c>
+      <c r="H6" t="n">
+        <v>156</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>15</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C7" t="n">
+        <v>57</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F7" t="n">
+        <v>14</v>
+      </c>
+      <c r="G7" t="n">
+        <v>138</v>
+      </c>
+      <c r="H7" t="n">
+        <v>156</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>15</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C8" t="n">
+        <v>57</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F8" t="n">
+        <v>14</v>
+      </c>
+      <c r="G8" t="n">
+        <v>138</v>
+      </c>
+      <c r="H8" t="n">
+        <v>156</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>15</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C9" t="n">
+        <v>57</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F9" t="n">
+        <v>14</v>
+      </c>
+      <c r="G9" t="n">
+        <v>138</v>
+      </c>
+      <c r="H9" t="n">
+        <v>156</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>15</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C10" t="n">
+        <v>57</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F10" t="n">
+        <v>14</v>
+      </c>
+      <c r="G10" t="n">
+        <v>138</v>
+      </c>
+      <c r="H10" t="n">
+        <v>156</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>15</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C11" t="n">
+        <v>57</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F11" t="n">
+        <v>14</v>
+      </c>
+      <c r="G11" t="n">
+        <v>138</v>
+      </c>
+      <c r="H11" t="n">
+        <v>156</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>15</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C12" t="n">
+        <v>57</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F12" t="n">
+        <v>14</v>
+      </c>
+      <c r="G12" t="n">
+        <v>138</v>
+      </c>
+      <c r="H12" t="n">
+        <v>156</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>15</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C13" t="n">
+        <v>57</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F13" t="n">
+        <v>14</v>
+      </c>
+      <c r="G13" t="n">
+        <v>138</v>
+      </c>
+      <c r="H13" t="n">
+        <v>156</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>15</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C14" t="n">
+        <v>57</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F14" t="n">
+        <v>14</v>
+      </c>
+      <c r="G14" t="n">
+        <v>138</v>
+      </c>
+      <c r="H14" t="n">
+        <v>156</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>15</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C15" t="n">
+        <v>57</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F15" t="n">
+        <v>14</v>
+      </c>
+      <c r="G15" t="n">
+        <v>138</v>
+      </c>
+      <c r="H15" t="n">
+        <v>156</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>15</v>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C16" t="n">
+        <v>57</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F16" t="n">
+        <v>14</v>
+      </c>
+      <c r="G16" t="n">
+        <v>138</v>
+      </c>
+      <c r="H16" t="n">
+        <v>156</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>15</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C17" t="n">
+        <v>57</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F17" t="n">
+        <v>14</v>
+      </c>
+      <c r="G17" t="n">
+        <v>138</v>
+      </c>
+      <c r="H17" t="n">
+        <v>156</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>15</v>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C18" t="n">
+        <v>57</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F18" t="n">
+        <v>14</v>
+      </c>
+      <c r="G18" t="n">
+        <v>138</v>
+      </c>
+      <c r="H18" t="n">
+        <v>156</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>15</v>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C19" t="n">
+        <v>57</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F19" t="n">
+        <v>14</v>
+      </c>
+      <c r="G19" t="n">
+        <v>138</v>
+      </c>
+      <c r="H19" t="n">
+        <v>156</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" t="n">
+        <v>15</v>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C20" t="n">
+        <v>57</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F20" t="n">
+        <v>14</v>
+      </c>
+      <c r="G20" t="n">
+        <v>138</v>
+      </c>
+      <c r="H20" t="n">
+        <v>156</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="n">
+        <v>15</v>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C21" t="n">
+        <v>57</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F21" t="n">
+        <v>14</v>
+      </c>
+      <c r="G21" t="n">
+        <v>138</v>
+      </c>
+      <c r="H21" t="n">
+        <v>156</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="n">
+        <v>15</v>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C22" t="n">
+        <v>57</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F22" t="n">
+        <v>14</v>
+      </c>
+      <c r="G22" t="n">
+        <v>138</v>
+      </c>
+      <c r="H22" t="n">
+        <v>156</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="n">
+        <v>15</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C23" t="n">
+        <v>57</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F23" t="n">
+        <v>14</v>
+      </c>
+      <c r="G23" t="n">
+        <v>138</v>
+      </c>
+      <c r="H23" t="n">
+        <v>156</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="n">
+        <v>15</v>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C24" t="n">
+        <v>57</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F24" t="n">
+        <v>14</v>
+      </c>
+      <c r="G24" t="n">
+        <v>138</v>
+      </c>
+      <c r="H24" t="n">
+        <v>156</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" t="n">
+        <v>15</v>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C25" t="n">
+        <v>57</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F25" t="n">
+        <v>14</v>
+      </c>
+      <c r="G25" t="n">
+        <v>138</v>
+      </c>
+      <c r="H25" t="n">
+        <v>156</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" t="n">
+        <v>15</v>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C26" t="n">
+        <v>57</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F26" t="n">
+        <v>14</v>
+      </c>
+      <c r="G26" t="n">
+        <v>138</v>
+      </c>
+      <c r="H26" t="n">
+        <v>156</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" t="n">
+        <v>15</v>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C27" t="n">
+        <v>57</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F27" t="n">
+        <v>14</v>
+      </c>
+      <c r="G27" t="n">
+        <v>138</v>
+      </c>
+      <c r="H27" t="n">
+        <v>156</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" t="n">
+        <v>15</v>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C28" t="n">
+        <v>57</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F28" t="n">
+        <v>14</v>
+      </c>
+      <c r="G28" t="n">
+        <v>138</v>
+      </c>
+      <c r="H28" t="n">
+        <v>156</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" t="n">
+        <v>15</v>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C29" t="n">
+        <v>57</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F29" t="n">
+        <v>14</v>
+      </c>
+      <c r="G29" t="n">
+        <v>138</v>
+      </c>
+      <c r="H29" t="n">
+        <v>156</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" t="n">
+        <v>15</v>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C30" t="n">
+        <v>57</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F30" t="n">
+        <v>14</v>
+      </c>
+      <c r="G30" t="n">
+        <v>138</v>
+      </c>
+      <c r="H30" t="n">
+        <v>156</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" t="n">
+        <v>15</v>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C31" t="n">
+        <v>57</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F31" t="n">
+        <v>14</v>
+      </c>
+      <c r="G31" t="n">
+        <v>138</v>
+      </c>
+      <c r="H31" t="n">
+        <v>156</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" t="n">
+        <v>15</v>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C32" t="n">
+        <v>57</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F32" t="n">
+        <v>14</v>
+      </c>
+      <c r="G32" t="n">
+        <v>138</v>
+      </c>
+      <c r="H32" t="n">
+        <v>156</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" t="n">
+        <v>15</v>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C33" t="n">
+        <v>57</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F33" t="n">
+        <v>14</v>
+      </c>
+      <c r="G33" t="n">
+        <v>138</v>
+      </c>
+      <c r="H33" t="n">
+        <v>156</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" t="n">
+        <v>15</v>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C34" t="n">
+        <v>57</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F34" t="n">
+        <v>14</v>
+      </c>
+      <c r="G34" t="n">
+        <v>138</v>
+      </c>
+      <c r="H34" t="n">
+        <v>156</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" t="n">
+        <v>15</v>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C35" t="n">
+        <v>57</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F35" t="n">
+        <v>14</v>
+      </c>
+      <c r="G35" t="n">
+        <v>138</v>
+      </c>
+      <c r="H35" t="n">
+        <v>156</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" t="n">
+        <v>15</v>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C36" t="n">
+        <v>57</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F36" t="n">
+        <v>14</v>
+      </c>
+      <c r="G36" t="n">
+        <v>138</v>
+      </c>
+      <c r="H36" t="n">
+        <v>156</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" t="n">
+        <v>15</v>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C37" t="n">
+        <v>57</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F37" t="n">
+        <v>14</v>
+      </c>
+      <c r="G37" t="n">
+        <v>138</v>
+      </c>
+      <c r="H37" t="n">
+        <v>156</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" t="n">
+        <v>15</v>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C38" t="n">
+        <v>57</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F38" t="n">
+        <v>14</v>
+      </c>
+      <c r="G38" t="n">
+        <v>138</v>
+      </c>
+      <c r="H38" t="n">
+        <v>156</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" t="n">
+        <v>15</v>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C39" t="n">
+        <v>57</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F39" t="n">
+        <v>14</v>
+      </c>
+      <c r="G39" t="n">
+        <v>138</v>
+      </c>
+      <c r="H39" t="n">
+        <v>156</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" t="n">
+        <v>15</v>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C40" t="n">
+        <v>57</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F40" t="n">
+        <v>14</v>
+      </c>
+      <c r="G40" t="n">
+        <v>138</v>
+      </c>
+      <c r="H40" t="n">
+        <v>156</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" t="n">
+        <v>15</v>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C41" t="n">
+        <v>57</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F41" t="n">
+        <v>14</v>
+      </c>
+      <c r="G41" t="n">
+        <v>138</v>
+      </c>
+      <c r="H41" t="n">
+        <v>156</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" t="n">
+        <v>15</v>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C42" t="n">
+        <v>57</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F42" t="n">
+        <v>14</v>
+      </c>
+      <c r="G42" t="n">
+        <v>138</v>
+      </c>
+      <c r="H42" t="n">
+        <v>156</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" t="n">
+        <v>15</v>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C43" t="n">
+        <v>57</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F43" t="n">
+        <v>14</v>
+      </c>
+      <c r="G43" t="n">
+        <v>138</v>
+      </c>
+      <c r="H43" t="n">
+        <v>156</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" t="n">
+        <v>15</v>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C44" t="n">
+        <v>57</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F44" t="n">
+        <v>14</v>
+      </c>
+      <c r="G44" t="n">
+        <v>138</v>
+      </c>
+      <c r="H44" t="n">
+        <v>156</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" t="n">
+        <v>15</v>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C45" t="n">
+        <v>57</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F45" t="n">
+        <v>14</v>
+      </c>
+      <c r="G45" t="n">
+        <v>138</v>
+      </c>
+      <c r="H45" t="n">
+        <v>156</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" t="n">
+        <v>15</v>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C46" t="n">
+        <v>57</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F46" t="n">
+        <v>14</v>
+      </c>
+      <c r="G46" t="n">
+        <v>138</v>
+      </c>
+      <c r="H46" t="n">
+        <v>156</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" t="n">
+        <v>15</v>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C47" t="n">
+        <v>57</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F47" t="n">
+        <v>14</v>
+      </c>
+      <c r="G47" t="n">
+        <v>138</v>
+      </c>
+      <c r="H47" t="n">
+        <v>156</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" t="n">
+        <v>15</v>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Game page now will load and create game.json file, whichever game is picked will be loaded. A game object will be created for whatever game is chosen
Need to figure out how to create player objects for every player in the game and add them to the excel sheet...
</commit_message>
<xml_diff>
--- a/player_stats.xlsx
+++ b/player_stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:L66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2611,6 +2611,880 @@
         </is>
       </c>
     </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C48" t="n">
+        <v>57</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F48" t="n">
+        <v>14</v>
+      </c>
+      <c r="G48" t="n">
+        <v>138</v>
+      </c>
+      <c r="H48" t="n">
+        <v>156</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" t="n">
+        <v>15</v>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C49" t="n">
+        <v>57</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F49" t="n">
+        <v>14</v>
+      </c>
+      <c r="G49" t="n">
+        <v>138</v>
+      </c>
+      <c r="H49" t="n">
+        <v>156</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" t="n">
+        <v>15</v>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C50" t="n">
+        <v>57</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F50" t="n">
+        <v>14</v>
+      </c>
+      <c r="G50" t="n">
+        <v>138</v>
+      </c>
+      <c r="H50" t="n">
+        <v>156</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" t="n">
+        <v>15</v>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C51" t="n">
+        <v>57</v>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F51" t="n">
+        <v>14</v>
+      </c>
+      <c r="G51" t="n">
+        <v>138</v>
+      </c>
+      <c r="H51" t="n">
+        <v>156</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J51" t="n">
+        <v>15</v>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>KAGS#7158</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C52" t="n">
+        <v>57</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F52" t="n">
+        <v>14</v>
+      </c>
+      <c r="G52" t="n">
+        <v>138</v>
+      </c>
+      <c r="H52" t="n">
+        <v>156</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0</v>
+      </c>
+      <c r="J52" t="n">
+        <v>15</v>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C53" t="n">
+        <v>57</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F53" t="n">
+        <v>14</v>
+      </c>
+      <c r="G53" t="n">
+        <v>138</v>
+      </c>
+      <c r="H53" t="n">
+        <v>156</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" t="n">
+        <v>15</v>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C54" t="n">
+        <v>57</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F54" t="n">
+        <v>14</v>
+      </c>
+      <c r="G54" t="n">
+        <v>138</v>
+      </c>
+      <c r="H54" t="n">
+        <v>156</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0</v>
+      </c>
+      <c r="J54" t="n">
+        <v>15</v>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C55" t="n">
+        <v>57</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F55" t="n">
+        <v>14</v>
+      </c>
+      <c r="G55" t="n">
+        <v>138</v>
+      </c>
+      <c r="H55" t="n">
+        <v>156</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0</v>
+      </c>
+      <c r="J55" t="n">
+        <v>15</v>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C56" t="n">
+        <v>57</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F56" t="n">
+        <v>14</v>
+      </c>
+      <c r="G56" t="n">
+        <v>138</v>
+      </c>
+      <c r="H56" t="n">
+        <v>156</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" t="n">
+        <v>15</v>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C57" t="n">
+        <v>57</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F57" t="n">
+        <v>14</v>
+      </c>
+      <c r="G57" t="n">
+        <v>138</v>
+      </c>
+      <c r="H57" t="n">
+        <v>156</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0</v>
+      </c>
+      <c r="J57" t="n">
+        <v>15</v>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C58" t="n">
+        <v>57</v>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F58" t="n">
+        <v>14</v>
+      </c>
+      <c r="G58" t="n">
+        <v>138</v>
+      </c>
+      <c r="H58" t="n">
+        <v>156</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" t="n">
+        <v>15</v>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C59" t="n">
+        <v>57</v>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F59" t="n">
+        <v>14</v>
+      </c>
+      <c r="G59" t="n">
+        <v>138</v>
+      </c>
+      <c r="H59" t="n">
+        <v>156</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0</v>
+      </c>
+      <c r="J59" t="n">
+        <v>15</v>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C60" t="n">
+        <v>57</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F60" t="n">
+        <v>14</v>
+      </c>
+      <c r="G60" t="n">
+        <v>138</v>
+      </c>
+      <c r="H60" t="n">
+        <v>156</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J60" t="n">
+        <v>15</v>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C61" t="n">
+        <v>57</v>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F61" t="n">
+        <v>14</v>
+      </c>
+      <c r="G61" t="n">
+        <v>138</v>
+      </c>
+      <c r="H61" t="n">
+        <v>156</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" t="n">
+        <v>15</v>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C62" t="n">
+        <v>57</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F62" t="n">
+        <v>14</v>
+      </c>
+      <c r="G62" t="n">
+        <v>138</v>
+      </c>
+      <c r="H62" t="n">
+        <v>156</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0</v>
+      </c>
+      <c r="J62" t="n">
+        <v>15</v>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C63" t="n">
+        <v>57</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F63" t="n">
+        <v>14</v>
+      </c>
+      <c r="G63" t="n">
+        <v>138</v>
+      </c>
+      <c r="H63" t="n">
+        <v>156</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0</v>
+      </c>
+      <c r="J63" t="n">
+        <v>15</v>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C64" t="n">
+        <v>57</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F64" t="n">
+        <v>14</v>
+      </c>
+      <c r="G64" t="n">
+        <v>138</v>
+      </c>
+      <c r="H64" t="n">
+        <v>156</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0</v>
+      </c>
+      <c r="J64" t="n">
+        <v>15</v>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C65" t="n">
+        <v>57</v>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F65" t="n">
+        <v>14</v>
+      </c>
+      <c r="G65" t="n">
+        <v>138</v>
+      </c>
+      <c r="H65" t="n">
+        <v>156</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0</v>
+      </c>
+      <c r="J65" t="n">
+        <v>15</v>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C66" t="n">
+        <v>57</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E66" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F66" t="n">
+        <v>14</v>
+      </c>
+      <c r="G66" t="n">
+        <v>138</v>
+      </c>
+      <c r="H66" t="n">
+        <v>156</v>
+      </c>
+      <c r="I66" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" t="n">
+        <v>15</v>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added ability to see multikills for a single game
</commit_message>
<xml_diff>
--- a/player_stats.xlsx
+++ b/player_stats.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L99"/>
+  <dimension ref="A1:L103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5003,6 +5003,190 @@
         </is>
       </c>
     </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C100" t="n">
+        <v>57</v>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E100" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F100" t="n">
+        <v>14</v>
+      </c>
+      <c r="G100" t="n">
+        <v>138</v>
+      </c>
+      <c r="H100" t="n">
+        <v>156</v>
+      </c>
+      <c r="I100" t="n">
+        <v>0</v>
+      </c>
+      <c r="J100" t="n">
+        <v>15</v>
+      </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L100" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C101" t="n">
+        <v>57</v>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E101" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F101" t="n">
+        <v>14</v>
+      </c>
+      <c r="G101" t="n">
+        <v>138</v>
+      </c>
+      <c r="H101" t="n">
+        <v>156</v>
+      </c>
+      <c r="I101" t="n">
+        <v>0</v>
+      </c>
+      <c r="J101" t="n">
+        <v>15</v>
+      </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L101" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C102" t="n">
+        <v>57</v>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E102" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F102" t="n">
+        <v>14</v>
+      </c>
+      <c r="G102" t="n">
+        <v>138</v>
+      </c>
+      <c r="H102" t="n">
+        <v>156</v>
+      </c>
+      <c r="I102" t="n">
+        <v>0</v>
+      </c>
+      <c r="J102" t="n">
+        <v>15</v>
+      </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L102" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C103" t="n">
+        <v>57</v>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E103" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F103" t="n">
+        <v>14</v>
+      </c>
+      <c r="G103" t="n">
+        <v>138</v>
+      </c>
+      <c r="H103" t="n">
+        <v>156</v>
+      </c>
+      <c r="I103" t="n">
+        <v>0</v>
+      </c>
+      <c r="J103" t="n">
+        <v>15</v>
+      </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L103" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Econ Class, Gets economy for each team for every round
Need to ass loss bonus and starting bonus's
</commit_message>
<xml_diff>
--- a/player_stats.xlsx
+++ b/player_stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L111"/>
+  <dimension ref="A1:L146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5555,6 +5555,1616 @@
         </is>
       </c>
     </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C112" t="n">
+        <v>57</v>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E112" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F112" t="n">
+        <v>14</v>
+      </c>
+      <c r="G112" t="n">
+        <v>138</v>
+      </c>
+      <c r="H112" t="n">
+        <v>156</v>
+      </c>
+      <c r="I112" t="n">
+        <v>0</v>
+      </c>
+      <c r="J112" t="n">
+        <v>15</v>
+      </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L112" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C113" t="n">
+        <v>57</v>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E113" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F113" t="n">
+        <v>14</v>
+      </c>
+      <c r="G113" t="n">
+        <v>138</v>
+      </c>
+      <c r="H113" t="n">
+        <v>156</v>
+      </c>
+      <c r="I113" t="n">
+        <v>0</v>
+      </c>
+      <c r="J113" t="n">
+        <v>15</v>
+      </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L113" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C114" t="n">
+        <v>57</v>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E114" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F114" t="n">
+        <v>14</v>
+      </c>
+      <c r="G114" t="n">
+        <v>138</v>
+      </c>
+      <c r="H114" t="n">
+        <v>156</v>
+      </c>
+      <c r="I114" t="n">
+        <v>0</v>
+      </c>
+      <c r="J114" t="n">
+        <v>15</v>
+      </c>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L114" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C115" t="n">
+        <v>57</v>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E115" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F115" t="n">
+        <v>14</v>
+      </c>
+      <c r="G115" t="n">
+        <v>138</v>
+      </c>
+      <c r="H115" t="n">
+        <v>156</v>
+      </c>
+      <c r="I115" t="n">
+        <v>0</v>
+      </c>
+      <c r="J115" t="n">
+        <v>15</v>
+      </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L115" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C116" t="n">
+        <v>57</v>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E116" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F116" t="n">
+        <v>14</v>
+      </c>
+      <c r="G116" t="n">
+        <v>138</v>
+      </c>
+      <c r="H116" t="n">
+        <v>156</v>
+      </c>
+      <c r="I116" t="n">
+        <v>0</v>
+      </c>
+      <c r="J116" t="n">
+        <v>15</v>
+      </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L116" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C117" t="n">
+        <v>57</v>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E117" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F117" t="n">
+        <v>14</v>
+      </c>
+      <c r="G117" t="n">
+        <v>138</v>
+      </c>
+      <c r="H117" t="n">
+        <v>156</v>
+      </c>
+      <c r="I117" t="n">
+        <v>0</v>
+      </c>
+      <c r="J117" t="n">
+        <v>15</v>
+      </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L117" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C118" t="n">
+        <v>57</v>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E118" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F118" t="n">
+        <v>14</v>
+      </c>
+      <c r="G118" t="n">
+        <v>138</v>
+      </c>
+      <c r="H118" t="n">
+        <v>156</v>
+      </c>
+      <c r="I118" t="n">
+        <v>0</v>
+      </c>
+      <c r="J118" t="n">
+        <v>15</v>
+      </c>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L118" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C119" t="n">
+        <v>57</v>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E119" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F119" t="n">
+        <v>14</v>
+      </c>
+      <c r="G119" t="n">
+        <v>138</v>
+      </c>
+      <c r="H119" t="n">
+        <v>156</v>
+      </c>
+      <c r="I119" t="n">
+        <v>0</v>
+      </c>
+      <c r="J119" t="n">
+        <v>15</v>
+      </c>
+      <c r="K119" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L119" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C120" t="n">
+        <v>57</v>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E120" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F120" t="n">
+        <v>14</v>
+      </c>
+      <c r="G120" t="n">
+        <v>138</v>
+      </c>
+      <c r="H120" t="n">
+        <v>156</v>
+      </c>
+      <c r="I120" t="n">
+        <v>0</v>
+      </c>
+      <c r="J120" t="n">
+        <v>15</v>
+      </c>
+      <c r="K120" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L120" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C121" t="n">
+        <v>57</v>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E121" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F121" t="n">
+        <v>14</v>
+      </c>
+      <c r="G121" t="n">
+        <v>138</v>
+      </c>
+      <c r="H121" t="n">
+        <v>156</v>
+      </c>
+      <c r="I121" t="n">
+        <v>0</v>
+      </c>
+      <c r="J121" t="n">
+        <v>15</v>
+      </c>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L121" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C122" t="n">
+        <v>57</v>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E122" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F122" t="n">
+        <v>14</v>
+      </c>
+      <c r="G122" t="n">
+        <v>138</v>
+      </c>
+      <c r="H122" t="n">
+        <v>156</v>
+      </c>
+      <c r="I122" t="n">
+        <v>0</v>
+      </c>
+      <c r="J122" t="n">
+        <v>15</v>
+      </c>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L122" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B123" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C123" t="n">
+        <v>57</v>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E123" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F123" t="n">
+        <v>14</v>
+      </c>
+      <c r="G123" t="n">
+        <v>138</v>
+      </c>
+      <c r="H123" t="n">
+        <v>156</v>
+      </c>
+      <c r="I123" t="n">
+        <v>0</v>
+      </c>
+      <c r="J123" t="n">
+        <v>15</v>
+      </c>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L123" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B124" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C124" t="n">
+        <v>57</v>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E124" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F124" t="n">
+        <v>14</v>
+      </c>
+      <c r="G124" t="n">
+        <v>138</v>
+      </c>
+      <c r="H124" t="n">
+        <v>156</v>
+      </c>
+      <c r="I124" t="n">
+        <v>0</v>
+      </c>
+      <c r="J124" t="n">
+        <v>15</v>
+      </c>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L124" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B125" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C125" t="n">
+        <v>57</v>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E125" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F125" t="n">
+        <v>14</v>
+      </c>
+      <c r="G125" t="n">
+        <v>138</v>
+      </c>
+      <c r="H125" t="n">
+        <v>156</v>
+      </c>
+      <c r="I125" t="n">
+        <v>0</v>
+      </c>
+      <c r="J125" t="n">
+        <v>15</v>
+      </c>
+      <c r="K125" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L125" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C126" t="n">
+        <v>57</v>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E126" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F126" t="n">
+        <v>14</v>
+      </c>
+      <c r="G126" t="n">
+        <v>138</v>
+      </c>
+      <c r="H126" t="n">
+        <v>156</v>
+      </c>
+      <c r="I126" t="n">
+        <v>0</v>
+      </c>
+      <c r="J126" t="n">
+        <v>15</v>
+      </c>
+      <c r="K126" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L126" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C127" t="n">
+        <v>57</v>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E127" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F127" t="n">
+        <v>14</v>
+      </c>
+      <c r="G127" t="n">
+        <v>138</v>
+      </c>
+      <c r="H127" t="n">
+        <v>156</v>
+      </c>
+      <c r="I127" t="n">
+        <v>0</v>
+      </c>
+      <c r="J127" t="n">
+        <v>15</v>
+      </c>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L127" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C128" t="n">
+        <v>57</v>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E128" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F128" t="n">
+        <v>14</v>
+      </c>
+      <c r="G128" t="n">
+        <v>138</v>
+      </c>
+      <c r="H128" t="n">
+        <v>156</v>
+      </c>
+      <c r="I128" t="n">
+        <v>0</v>
+      </c>
+      <c r="J128" t="n">
+        <v>15</v>
+      </c>
+      <c r="K128" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L128" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C129" t="n">
+        <v>57</v>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E129" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F129" t="n">
+        <v>14</v>
+      </c>
+      <c r="G129" t="n">
+        <v>138</v>
+      </c>
+      <c r="H129" t="n">
+        <v>156</v>
+      </c>
+      <c r="I129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J129" t="n">
+        <v>15</v>
+      </c>
+      <c r="K129" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L129" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C130" t="n">
+        <v>57</v>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E130" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F130" t="n">
+        <v>14</v>
+      </c>
+      <c r="G130" t="n">
+        <v>138</v>
+      </c>
+      <c r="H130" t="n">
+        <v>156</v>
+      </c>
+      <c r="I130" t="n">
+        <v>0</v>
+      </c>
+      <c r="J130" t="n">
+        <v>15</v>
+      </c>
+      <c r="K130" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L130" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B131" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C131" t="n">
+        <v>57</v>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E131" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F131" t="n">
+        <v>14</v>
+      </c>
+      <c r="G131" t="n">
+        <v>138</v>
+      </c>
+      <c r="H131" t="n">
+        <v>156</v>
+      </c>
+      <c r="I131" t="n">
+        <v>0</v>
+      </c>
+      <c r="J131" t="n">
+        <v>15</v>
+      </c>
+      <c r="K131" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L131" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B132" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C132" t="n">
+        <v>57</v>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E132" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F132" t="n">
+        <v>14</v>
+      </c>
+      <c r="G132" t="n">
+        <v>138</v>
+      </c>
+      <c r="H132" t="n">
+        <v>156</v>
+      </c>
+      <c r="I132" t="n">
+        <v>0</v>
+      </c>
+      <c r="J132" t="n">
+        <v>15</v>
+      </c>
+      <c r="K132" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L132" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B133" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C133" t="n">
+        <v>57</v>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E133" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F133" t="n">
+        <v>14</v>
+      </c>
+      <c r="G133" t="n">
+        <v>138</v>
+      </c>
+      <c r="H133" t="n">
+        <v>156</v>
+      </c>
+      <c r="I133" t="n">
+        <v>0</v>
+      </c>
+      <c r="J133" t="n">
+        <v>15</v>
+      </c>
+      <c r="K133" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L133" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B134" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C134" t="n">
+        <v>57</v>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E134" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F134" t="n">
+        <v>14</v>
+      </c>
+      <c r="G134" t="n">
+        <v>138</v>
+      </c>
+      <c r="H134" t="n">
+        <v>156</v>
+      </c>
+      <c r="I134" t="n">
+        <v>0</v>
+      </c>
+      <c r="J134" t="n">
+        <v>15</v>
+      </c>
+      <c r="K134" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L134" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B135" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C135" t="n">
+        <v>57</v>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E135" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F135" t="n">
+        <v>14</v>
+      </c>
+      <c r="G135" t="n">
+        <v>138</v>
+      </c>
+      <c r="H135" t="n">
+        <v>156</v>
+      </c>
+      <c r="I135" t="n">
+        <v>0</v>
+      </c>
+      <c r="J135" t="n">
+        <v>15</v>
+      </c>
+      <c r="K135" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L135" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B136" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C136" t="n">
+        <v>57</v>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E136" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F136" t="n">
+        <v>14</v>
+      </c>
+      <c r="G136" t="n">
+        <v>138</v>
+      </c>
+      <c r="H136" t="n">
+        <v>156</v>
+      </c>
+      <c r="I136" t="n">
+        <v>0</v>
+      </c>
+      <c r="J136" t="n">
+        <v>15</v>
+      </c>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L136" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C137" t="n">
+        <v>57</v>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E137" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F137" t="n">
+        <v>14</v>
+      </c>
+      <c r="G137" t="n">
+        <v>138</v>
+      </c>
+      <c r="H137" t="n">
+        <v>156</v>
+      </c>
+      <c r="I137" t="n">
+        <v>0</v>
+      </c>
+      <c r="J137" t="n">
+        <v>15</v>
+      </c>
+      <c r="K137" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L137" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B138" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C138" t="n">
+        <v>57</v>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E138" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F138" t="n">
+        <v>14</v>
+      </c>
+      <c r="G138" t="n">
+        <v>138</v>
+      </c>
+      <c r="H138" t="n">
+        <v>156</v>
+      </c>
+      <c r="I138" t="n">
+        <v>0</v>
+      </c>
+      <c r="J138" t="n">
+        <v>15</v>
+      </c>
+      <c r="K138" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L138" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C139" t="n">
+        <v>57</v>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E139" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F139" t="n">
+        <v>14</v>
+      </c>
+      <c r="G139" t="n">
+        <v>138</v>
+      </c>
+      <c r="H139" t="n">
+        <v>156</v>
+      </c>
+      <c r="I139" t="n">
+        <v>0</v>
+      </c>
+      <c r="J139" t="n">
+        <v>15</v>
+      </c>
+      <c r="K139" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L139" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C140" t="n">
+        <v>57</v>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E140" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F140" t="n">
+        <v>14</v>
+      </c>
+      <c r="G140" t="n">
+        <v>138</v>
+      </c>
+      <c r="H140" t="n">
+        <v>156</v>
+      </c>
+      <c r="I140" t="n">
+        <v>0</v>
+      </c>
+      <c r="J140" t="n">
+        <v>15</v>
+      </c>
+      <c r="K140" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L140" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B141" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C141" t="n">
+        <v>57</v>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E141" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F141" t="n">
+        <v>14</v>
+      </c>
+      <c r="G141" t="n">
+        <v>138</v>
+      </c>
+      <c r="H141" t="n">
+        <v>156</v>
+      </c>
+      <c r="I141" t="n">
+        <v>0</v>
+      </c>
+      <c r="J141" t="n">
+        <v>15</v>
+      </c>
+      <c r="K141" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L141" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B142" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C142" t="n">
+        <v>57</v>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E142" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F142" t="n">
+        <v>14</v>
+      </c>
+      <c r="G142" t="n">
+        <v>138</v>
+      </c>
+      <c r="H142" t="n">
+        <v>156</v>
+      </c>
+      <c r="I142" t="n">
+        <v>0</v>
+      </c>
+      <c r="J142" t="n">
+        <v>15</v>
+      </c>
+      <c r="K142" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L142" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B143" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C143" t="n">
+        <v>57</v>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E143" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F143" t="n">
+        <v>14</v>
+      </c>
+      <c r="G143" t="n">
+        <v>138</v>
+      </c>
+      <c r="H143" t="n">
+        <v>156</v>
+      </c>
+      <c r="I143" t="n">
+        <v>0</v>
+      </c>
+      <c r="J143" t="n">
+        <v>15</v>
+      </c>
+      <c r="K143" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L143" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B144" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C144" t="n">
+        <v>57</v>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E144" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F144" t="n">
+        <v>14</v>
+      </c>
+      <c r="G144" t="n">
+        <v>138</v>
+      </c>
+      <c r="H144" t="n">
+        <v>156</v>
+      </c>
+      <c r="I144" t="n">
+        <v>0</v>
+      </c>
+      <c r="J144" t="n">
+        <v>15</v>
+      </c>
+      <c r="K144" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L144" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B145" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C145" t="n">
+        <v>57</v>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E145" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F145" t="n">
+        <v>14</v>
+      </c>
+      <c r="G145" t="n">
+        <v>138</v>
+      </c>
+      <c r="H145" t="n">
+        <v>156</v>
+      </c>
+      <c r="I145" t="n">
+        <v>0</v>
+      </c>
+      <c r="J145" t="n">
+        <v>15</v>
+      </c>
+      <c r="K145" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L145" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B146" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C146" t="n">
+        <v>57</v>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E146" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F146" t="n">
+        <v>14</v>
+      </c>
+      <c r="G146" t="n">
+        <v>138</v>
+      </c>
+      <c r="H146" t="n">
+        <v>156</v>
+      </c>
+      <c r="I146" t="n">
+        <v>0</v>
+      </c>
+      <c r="J146" t="n">
+        <v>15</v>
+      </c>
+      <c r="K146" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L146" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added econ graph, and red team accuracy graph, need to do blue team and figure out label stuff
</commit_message>
<xml_diff>
--- a/player_stats.xlsx
+++ b/player_stats.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L153"/>
+  <dimension ref="A1:L197"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7487,6 +7487,2030 @@
         </is>
       </c>
     </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B154" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C154" t="n">
+        <v>57</v>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E154" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F154" t="n">
+        <v>14</v>
+      </c>
+      <c r="G154" t="n">
+        <v>138</v>
+      </c>
+      <c r="H154" t="n">
+        <v>156</v>
+      </c>
+      <c r="I154" t="n">
+        <v>0</v>
+      </c>
+      <c r="J154" t="n">
+        <v>15</v>
+      </c>
+      <c r="K154" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L154" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B155" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C155" t="n">
+        <v>57</v>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E155" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F155" t="n">
+        <v>14</v>
+      </c>
+      <c r="G155" t="n">
+        <v>138</v>
+      </c>
+      <c r="H155" t="n">
+        <v>156</v>
+      </c>
+      <c r="I155" t="n">
+        <v>0</v>
+      </c>
+      <c r="J155" t="n">
+        <v>15</v>
+      </c>
+      <c r="K155" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L155" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B156" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C156" t="n">
+        <v>57</v>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E156" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F156" t="n">
+        <v>14</v>
+      </c>
+      <c r="G156" t="n">
+        <v>138</v>
+      </c>
+      <c r="H156" t="n">
+        <v>156</v>
+      </c>
+      <c r="I156" t="n">
+        <v>0</v>
+      </c>
+      <c r="J156" t="n">
+        <v>15</v>
+      </c>
+      <c r="K156" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L156" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B157" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C157" t="n">
+        <v>57</v>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E157" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F157" t="n">
+        <v>14</v>
+      </c>
+      <c r="G157" t="n">
+        <v>138</v>
+      </c>
+      <c r="H157" t="n">
+        <v>156</v>
+      </c>
+      <c r="I157" t="n">
+        <v>0</v>
+      </c>
+      <c r="J157" t="n">
+        <v>15</v>
+      </c>
+      <c r="K157" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L157" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B158" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C158" t="n">
+        <v>57</v>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E158" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F158" t="n">
+        <v>14</v>
+      </c>
+      <c r="G158" t="n">
+        <v>138</v>
+      </c>
+      <c r="H158" t="n">
+        <v>156</v>
+      </c>
+      <c r="I158" t="n">
+        <v>0</v>
+      </c>
+      <c r="J158" t="n">
+        <v>15</v>
+      </c>
+      <c r="K158" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L158" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B159" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C159" t="n">
+        <v>57</v>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E159" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F159" t="n">
+        <v>14</v>
+      </c>
+      <c r="G159" t="n">
+        <v>138</v>
+      </c>
+      <c r="H159" t="n">
+        <v>156</v>
+      </c>
+      <c r="I159" t="n">
+        <v>0</v>
+      </c>
+      <c r="J159" t="n">
+        <v>15</v>
+      </c>
+      <c r="K159" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L159" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B160" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C160" t="n">
+        <v>57</v>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E160" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F160" t="n">
+        <v>14</v>
+      </c>
+      <c r="G160" t="n">
+        <v>138</v>
+      </c>
+      <c r="H160" t="n">
+        <v>156</v>
+      </c>
+      <c r="I160" t="n">
+        <v>0</v>
+      </c>
+      <c r="J160" t="n">
+        <v>15</v>
+      </c>
+      <c r="K160" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L160" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B161" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C161" t="n">
+        <v>57</v>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E161" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F161" t="n">
+        <v>14</v>
+      </c>
+      <c r="G161" t="n">
+        <v>138</v>
+      </c>
+      <c r="H161" t="n">
+        <v>156</v>
+      </c>
+      <c r="I161" t="n">
+        <v>0</v>
+      </c>
+      <c r="J161" t="n">
+        <v>15</v>
+      </c>
+      <c r="K161" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L161" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B162" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C162" t="n">
+        <v>57</v>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E162" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F162" t="n">
+        <v>14</v>
+      </c>
+      <c r="G162" t="n">
+        <v>138</v>
+      </c>
+      <c r="H162" t="n">
+        <v>156</v>
+      </c>
+      <c r="I162" t="n">
+        <v>0</v>
+      </c>
+      <c r="J162" t="n">
+        <v>15</v>
+      </c>
+      <c r="K162" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L162" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B163" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C163" t="n">
+        <v>57</v>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E163" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F163" t="n">
+        <v>14</v>
+      </c>
+      <c r="G163" t="n">
+        <v>138</v>
+      </c>
+      <c r="H163" t="n">
+        <v>156</v>
+      </c>
+      <c r="I163" t="n">
+        <v>0</v>
+      </c>
+      <c r="J163" t="n">
+        <v>15</v>
+      </c>
+      <c r="K163" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L163" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B164" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C164" t="n">
+        <v>57</v>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E164" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F164" t="n">
+        <v>14</v>
+      </c>
+      <c r="G164" t="n">
+        <v>138</v>
+      </c>
+      <c r="H164" t="n">
+        <v>156</v>
+      </c>
+      <c r="I164" t="n">
+        <v>0</v>
+      </c>
+      <c r="J164" t="n">
+        <v>15</v>
+      </c>
+      <c r="K164" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L164" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B165" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C165" t="n">
+        <v>57</v>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E165" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F165" t="n">
+        <v>14</v>
+      </c>
+      <c r="G165" t="n">
+        <v>138</v>
+      </c>
+      <c r="H165" t="n">
+        <v>156</v>
+      </c>
+      <c r="I165" t="n">
+        <v>0</v>
+      </c>
+      <c r="J165" t="n">
+        <v>15</v>
+      </c>
+      <c r="K165" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L165" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>vora #xyz</t>
+        </is>
+      </c>
+      <c r="B166" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="C166" t="n">
+        <v>66</v>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>Sova</t>
+        </is>
+      </c>
+      <c r="E166" t="n">
+        <v>34.1</v>
+      </c>
+      <c r="F166" t="n">
+        <v>77</v>
+      </c>
+      <c r="G166" t="n">
+        <v>249</v>
+      </c>
+      <c r="H166" t="n">
+        <v>124</v>
+      </c>
+      <c r="I166" t="n">
+        <v>0</v>
+      </c>
+      <c r="J166" t="n">
+        <v>65</v>
+      </c>
+      <c r="K166" t="inlineStr">
+        <is>
+          <t>Lead</t>
+        </is>
+      </c>
+      <c r="L166" t="inlineStr">
+        <is>
+          <t>['Clutch King', 'Engager', 'Sniper', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>twitch nightz1x #aim</t>
+        </is>
+      </c>
+      <c r="B167" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="C167" t="n">
+        <v>59</v>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>Clove</t>
+        </is>
+      </c>
+      <c r="E167" t="n">
+        <v>40.6</v>
+      </c>
+      <c r="F167" t="n">
+        <v>50</v>
+      </c>
+      <c r="G167" t="n">
+        <v>454</v>
+      </c>
+      <c r="H167" t="n">
+        <v>381</v>
+      </c>
+      <c r="I167" t="n">
+        <v>0</v>
+      </c>
+      <c r="J167" t="n">
+        <v>81</v>
+      </c>
+      <c r="K167" t="inlineStr">
+        <is>
+          <t>Zinc</t>
+        </is>
+      </c>
+      <c r="L167" t="inlineStr">
+        <is>
+          <t>['Engager', 'Sniper', 'Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>rookie #aimer</t>
+        </is>
+      </c>
+      <c r="B168" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="C168" t="n">
+        <v>51</v>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>Chamber</t>
+        </is>
+      </c>
+      <c r="E168" t="n">
+        <v>32</v>
+      </c>
+      <c r="F168" t="n">
+        <v>51</v>
+      </c>
+      <c r="G168" t="n">
+        <v>246</v>
+      </c>
+      <c r="H168" t="n">
+        <v>226</v>
+      </c>
+      <c r="I168" t="n">
+        <v>0</v>
+      </c>
+      <c r="J168" t="n">
+        <v>4</v>
+      </c>
+      <c r="K168" t="inlineStr">
+        <is>
+          <t>Palladium</t>
+        </is>
+      </c>
+      <c r="L168" t="inlineStr">
+        <is>
+          <t>['Clutch King', 'Engager', 'Sniper', 'Rusher']</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>tyd #jobab</t>
+        </is>
+      </c>
+      <c r="B169" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="C169" t="n">
+        <v>51</v>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>Clove</t>
+        </is>
+      </c>
+      <c r="E169" t="n">
+        <v>36.9</v>
+      </c>
+      <c r="F169" t="n">
+        <v>55</v>
+      </c>
+      <c r="G169" t="n">
+        <v>290</v>
+      </c>
+      <c r="H169" t="n">
+        <v>281</v>
+      </c>
+      <c r="I169" t="n">
+        <v>0</v>
+      </c>
+      <c r="J169" t="n">
+        <v>39</v>
+      </c>
+      <c r="K169" t="inlineStr">
+        <is>
+          <t>Palladium</t>
+        </is>
+      </c>
+      <c r="L169" t="inlineStr">
+        <is>
+          <t>['Clutch King', 'Engager', 'Sniper', 'Rusher']</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B170" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C170" t="n">
+        <v>57</v>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E170" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F170" t="n">
+        <v>14</v>
+      </c>
+      <c r="G170" t="n">
+        <v>138</v>
+      </c>
+      <c r="H170" t="n">
+        <v>156</v>
+      </c>
+      <c r="I170" t="n">
+        <v>0</v>
+      </c>
+      <c r="J170" t="n">
+        <v>15</v>
+      </c>
+      <c r="K170" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L170" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B171" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C171" t="n">
+        <v>57</v>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E171" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F171" t="n">
+        <v>14</v>
+      </c>
+      <c r="G171" t="n">
+        <v>138</v>
+      </c>
+      <c r="H171" t="n">
+        <v>156</v>
+      </c>
+      <c r="I171" t="n">
+        <v>0</v>
+      </c>
+      <c r="J171" t="n">
+        <v>15</v>
+      </c>
+      <c r="K171" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L171" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B172" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C172" t="n">
+        <v>57</v>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E172" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F172" t="n">
+        <v>14</v>
+      </c>
+      <c r="G172" t="n">
+        <v>138</v>
+      </c>
+      <c r="H172" t="n">
+        <v>156</v>
+      </c>
+      <c r="I172" t="n">
+        <v>0</v>
+      </c>
+      <c r="J172" t="n">
+        <v>15</v>
+      </c>
+      <c r="K172" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L172" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B173" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C173" t="n">
+        <v>57</v>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E173" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F173" t="n">
+        <v>14</v>
+      </c>
+      <c r="G173" t="n">
+        <v>138</v>
+      </c>
+      <c r="H173" t="n">
+        <v>156</v>
+      </c>
+      <c r="I173" t="n">
+        <v>0</v>
+      </c>
+      <c r="J173" t="n">
+        <v>15</v>
+      </c>
+      <c r="K173" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L173" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B174" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C174" t="n">
+        <v>57</v>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E174" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F174" t="n">
+        <v>14</v>
+      </c>
+      <c r="G174" t="n">
+        <v>138</v>
+      </c>
+      <c r="H174" t="n">
+        <v>156</v>
+      </c>
+      <c r="I174" t="n">
+        <v>0</v>
+      </c>
+      <c r="J174" t="n">
+        <v>15</v>
+      </c>
+      <c r="K174" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L174" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B175" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C175" t="n">
+        <v>57</v>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E175" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F175" t="n">
+        <v>14</v>
+      </c>
+      <c r="G175" t="n">
+        <v>138</v>
+      </c>
+      <c r="H175" t="n">
+        <v>156</v>
+      </c>
+      <c r="I175" t="n">
+        <v>0</v>
+      </c>
+      <c r="J175" t="n">
+        <v>15</v>
+      </c>
+      <c r="K175" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L175" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B176" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C176" t="n">
+        <v>57</v>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E176" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F176" t="n">
+        <v>14</v>
+      </c>
+      <c r="G176" t="n">
+        <v>138</v>
+      </c>
+      <c r="H176" t="n">
+        <v>156</v>
+      </c>
+      <c r="I176" t="n">
+        <v>0</v>
+      </c>
+      <c r="J176" t="n">
+        <v>15</v>
+      </c>
+      <c r="K176" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L176" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B177" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C177" t="n">
+        <v>57</v>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E177" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F177" t="n">
+        <v>14</v>
+      </c>
+      <c r="G177" t="n">
+        <v>138</v>
+      </c>
+      <c r="H177" t="n">
+        <v>156</v>
+      </c>
+      <c r="I177" t="n">
+        <v>0</v>
+      </c>
+      <c r="J177" t="n">
+        <v>15</v>
+      </c>
+      <c r="K177" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L177" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B178" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C178" t="n">
+        <v>57</v>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E178" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F178" t="n">
+        <v>14</v>
+      </c>
+      <c r="G178" t="n">
+        <v>138</v>
+      </c>
+      <c r="H178" t="n">
+        <v>156</v>
+      </c>
+      <c r="I178" t="n">
+        <v>0</v>
+      </c>
+      <c r="J178" t="n">
+        <v>15</v>
+      </c>
+      <c r="K178" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L178" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B179" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C179" t="n">
+        <v>57</v>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E179" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F179" t="n">
+        <v>14</v>
+      </c>
+      <c r="G179" t="n">
+        <v>138</v>
+      </c>
+      <c r="H179" t="n">
+        <v>156</v>
+      </c>
+      <c r="I179" t="n">
+        <v>0</v>
+      </c>
+      <c r="J179" t="n">
+        <v>15</v>
+      </c>
+      <c r="K179" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L179" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B180" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C180" t="n">
+        <v>57</v>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E180" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F180" t="n">
+        <v>14</v>
+      </c>
+      <c r="G180" t="n">
+        <v>138</v>
+      </c>
+      <c r="H180" t="n">
+        <v>156</v>
+      </c>
+      <c r="I180" t="n">
+        <v>0</v>
+      </c>
+      <c r="J180" t="n">
+        <v>15</v>
+      </c>
+      <c r="K180" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L180" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B181" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C181" t="n">
+        <v>57</v>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E181" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F181" t="n">
+        <v>14</v>
+      </c>
+      <c r="G181" t="n">
+        <v>138</v>
+      </c>
+      <c r="H181" t="n">
+        <v>156</v>
+      </c>
+      <c r="I181" t="n">
+        <v>0</v>
+      </c>
+      <c r="J181" t="n">
+        <v>15</v>
+      </c>
+      <c r="K181" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L181" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B182" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C182" t="n">
+        <v>57</v>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E182" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F182" t="n">
+        <v>14</v>
+      </c>
+      <c r="G182" t="n">
+        <v>138</v>
+      </c>
+      <c r="H182" t="n">
+        <v>156</v>
+      </c>
+      <c r="I182" t="n">
+        <v>0</v>
+      </c>
+      <c r="J182" t="n">
+        <v>15</v>
+      </c>
+      <c r="K182" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L182" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B183" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C183" t="n">
+        <v>57</v>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E183" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F183" t="n">
+        <v>14</v>
+      </c>
+      <c r="G183" t="n">
+        <v>138</v>
+      </c>
+      <c r="H183" t="n">
+        <v>156</v>
+      </c>
+      <c r="I183" t="n">
+        <v>0</v>
+      </c>
+      <c r="J183" t="n">
+        <v>15</v>
+      </c>
+      <c r="K183" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L183" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B184" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C184" t="n">
+        <v>57</v>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E184" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F184" t="n">
+        <v>14</v>
+      </c>
+      <c r="G184" t="n">
+        <v>138</v>
+      </c>
+      <c r="H184" t="n">
+        <v>156</v>
+      </c>
+      <c r="I184" t="n">
+        <v>0</v>
+      </c>
+      <c r="J184" t="n">
+        <v>15</v>
+      </c>
+      <c r="K184" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L184" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B185" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C185" t="n">
+        <v>57</v>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E185" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F185" t="n">
+        <v>14</v>
+      </c>
+      <c r="G185" t="n">
+        <v>138</v>
+      </c>
+      <c r="H185" t="n">
+        <v>156</v>
+      </c>
+      <c r="I185" t="n">
+        <v>0</v>
+      </c>
+      <c r="J185" t="n">
+        <v>15</v>
+      </c>
+      <c r="K185" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L185" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B186" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C186" t="n">
+        <v>57</v>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E186" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F186" t="n">
+        <v>14</v>
+      </c>
+      <c r="G186" t="n">
+        <v>138</v>
+      </c>
+      <c r="H186" t="n">
+        <v>156</v>
+      </c>
+      <c r="I186" t="n">
+        <v>0</v>
+      </c>
+      <c r="J186" t="n">
+        <v>15</v>
+      </c>
+      <c r="K186" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L186" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B187" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C187" t="n">
+        <v>57</v>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E187" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F187" t="n">
+        <v>14</v>
+      </c>
+      <c r="G187" t="n">
+        <v>138</v>
+      </c>
+      <c r="H187" t="n">
+        <v>156</v>
+      </c>
+      <c r="I187" t="n">
+        <v>0</v>
+      </c>
+      <c r="J187" t="n">
+        <v>15</v>
+      </c>
+      <c r="K187" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L187" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B188" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C188" t="n">
+        <v>57</v>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E188" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F188" t="n">
+        <v>14</v>
+      </c>
+      <c r="G188" t="n">
+        <v>138</v>
+      </c>
+      <c r="H188" t="n">
+        <v>156</v>
+      </c>
+      <c r="I188" t="n">
+        <v>0</v>
+      </c>
+      <c r="J188" t="n">
+        <v>15</v>
+      </c>
+      <c r="K188" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L188" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B189" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C189" t="n">
+        <v>57</v>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E189" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F189" t="n">
+        <v>14</v>
+      </c>
+      <c r="G189" t="n">
+        <v>138</v>
+      </c>
+      <c r="H189" t="n">
+        <v>156</v>
+      </c>
+      <c r="I189" t="n">
+        <v>0</v>
+      </c>
+      <c r="J189" t="n">
+        <v>15</v>
+      </c>
+      <c r="K189" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L189" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B190" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C190" t="n">
+        <v>57</v>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E190" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F190" t="n">
+        <v>14</v>
+      </c>
+      <c r="G190" t="n">
+        <v>138</v>
+      </c>
+      <c r="H190" t="n">
+        <v>156</v>
+      </c>
+      <c r="I190" t="n">
+        <v>0</v>
+      </c>
+      <c r="J190" t="n">
+        <v>15</v>
+      </c>
+      <c r="K190" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L190" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B191" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C191" t="n">
+        <v>57</v>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E191" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F191" t="n">
+        <v>14</v>
+      </c>
+      <c r="G191" t="n">
+        <v>138</v>
+      </c>
+      <c r="H191" t="n">
+        <v>156</v>
+      </c>
+      <c r="I191" t="n">
+        <v>0</v>
+      </c>
+      <c r="J191" t="n">
+        <v>15</v>
+      </c>
+      <c r="K191" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L191" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B192" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C192" t="n">
+        <v>57</v>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E192" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F192" t="n">
+        <v>14</v>
+      </c>
+      <c r="G192" t="n">
+        <v>138</v>
+      </c>
+      <c r="H192" t="n">
+        <v>156</v>
+      </c>
+      <c r="I192" t="n">
+        <v>0</v>
+      </c>
+      <c r="J192" t="n">
+        <v>15</v>
+      </c>
+      <c r="K192" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L192" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B193" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C193" t="n">
+        <v>57</v>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E193" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F193" t="n">
+        <v>14</v>
+      </c>
+      <c r="G193" t="n">
+        <v>138</v>
+      </c>
+      <c r="H193" t="n">
+        <v>156</v>
+      </c>
+      <c r="I193" t="n">
+        <v>0</v>
+      </c>
+      <c r="J193" t="n">
+        <v>15</v>
+      </c>
+      <c r="K193" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L193" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B194" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C194" t="n">
+        <v>57</v>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E194" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F194" t="n">
+        <v>14</v>
+      </c>
+      <c r="G194" t="n">
+        <v>138</v>
+      </c>
+      <c r="H194" t="n">
+        <v>156</v>
+      </c>
+      <c r="I194" t="n">
+        <v>0</v>
+      </c>
+      <c r="J194" t="n">
+        <v>15</v>
+      </c>
+      <c r="K194" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L194" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B195" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C195" t="n">
+        <v>57</v>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E195" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F195" t="n">
+        <v>14</v>
+      </c>
+      <c r="G195" t="n">
+        <v>138</v>
+      </c>
+      <c r="H195" t="n">
+        <v>156</v>
+      </c>
+      <c r="I195" t="n">
+        <v>0</v>
+      </c>
+      <c r="J195" t="n">
+        <v>15</v>
+      </c>
+      <c r="K195" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L195" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B196" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C196" t="n">
+        <v>57</v>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E196" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F196" t="n">
+        <v>14</v>
+      </c>
+      <c r="G196" t="n">
+        <v>138</v>
+      </c>
+      <c r="H196" t="n">
+        <v>156</v>
+      </c>
+      <c r="I196" t="n">
+        <v>0</v>
+      </c>
+      <c r="J196" t="n">
+        <v>15</v>
+      </c>
+      <c r="K196" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L196" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>KAGS #7158</t>
+        </is>
+      </c>
+      <c r="B197" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="C197" t="n">
+        <v>57</v>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>Jett</t>
+        </is>
+      </c>
+      <c r="E197" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F197" t="n">
+        <v>14</v>
+      </c>
+      <c r="G197" t="n">
+        <v>138</v>
+      </c>
+      <c r="H197" t="n">
+        <v>156</v>
+      </c>
+      <c r="I197" t="n">
+        <v>0</v>
+      </c>
+      <c r="J197" t="n">
+        <v>15</v>
+      </c>
+      <c r="K197" t="inlineStr">
+        <is>
+          <t>Nickel</t>
+        </is>
+      </c>
+      <c r="L197" t="inlineStr">
+        <is>
+          <t>['Rusher', 'Straight Up Winner']</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>